<commit_message>
report file is added
</commit_message>
<xml_diff>
--- a/new_modules/Summary_2022-08-05_L2A.xlsx
+++ b/new_modules/Summary_2022-08-05_L2A.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.0516</v>
+        <v>0.3254</v>
       </c>
       <c r="C2">
-        <v>-0.0516</v>
+        <v>0.3254</v>
       </c>
       <c r="D2">
-        <v>-0.06950000000000001</v>
+        <v>0.3086000084877014</v>
       </c>
       <c r="E2">
-        <v>0.1671</v>
+        <v>0.5224000215530396</v>
       </c>
       <c r="F2">
-        <v>-0.1994</v>
+        <v>0.1756999939680099</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.07870000000000001</v>
+        <v>0.3977</v>
       </c>
       <c r="C3">
-        <v>-0.07870000000000001</v>
+        <v>0.3977</v>
       </c>
       <c r="D3">
-        <v>-0.09229999999999999</v>
+        <v>0.4076</v>
       </c>
       <c r="E3">
-        <v>0.2385</v>
+        <v>0.6488999724388123</v>
       </c>
       <c r="F3">
-        <v>-0.3038</v>
+        <v>0.1066000014543533</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.0529</v>
+        <v>0.3857</v>
       </c>
       <c r="C4">
-        <v>-0.0529</v>
+        <v>0.3857</v>
       </c>
       <c r="D4">
-        <v>-0.0592</v>
+        <v>0.3877</v>
       </c>
       <c r="E4">
-        <v>0.1589</v>
+        <v>0.503600001335144</v>
       </c>
       <c r="F4">
-        <v>-0.1585</v>
+        <v>0.1861999928951263</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0829</v>
+        <v>0.2531</v>
       </c>
       <c r="C5">
-        <v>0.0829</v>
+        <v>0.2531</v>
       </c>
       <c r="D5">
-        <v>0.1022</v>
+        <v>0.2237</v>
       </c>
       <c r="E5">
-        <v>0.2467</v>
+        <v>0.4767000079154968</v>
       </c>
       <c r="F5">
-        <v>-0.1316</v>
+        <v>0.09839999675750732</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.06469999999999999</v>
+        <v>0.2696</v>
       </c>
       <c r="C6">
-        <v>0.06469999999999999</v>
+        <v>0.2696</v>
       </c>
       <c r="D6">
-        <v>0.0582</v>
+        <v>0.2793</v>
       </c>
       <c r="E6">
-        <v>0.2309</v>
+        <v>0.4860999882221222</v>
       </c>
       <c r="F6">
-        <v>-0.1409</v>
+        <v>0.1142000034451485</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.0282</v>
+        <v>0.2953</v>
       </c>
       <c r="C7">
-        <v>0.0282</v>
+        <v>0.2953</v>
       </c>
       <c r="D7">
-        <v>0.0283</v>
+        <v>0.3003999888896942</v>
       </c>
       <c r="E7">
-        <v>0.1495</v>
+        <v>0.3982000052928925</v>
       </c>
       <c r="F7">
-        <v>-0.1147</v>
+        <v>0.1956000030040741</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.0249</v>
+        <v>0.2883</v>
       </c>
       <c r="C8">
-        <v>0.0249</v>
+        <v>0.2883</v>
       </c>
       <c r="D8">
-        <v>0.0249</v>
+        <v>0.287</v>
       </c>
       <c r="E8">
-        <v>0.1495</v>
+        <v>0.4081999957561493</v>
       </c>
       <c r="F8">
-        <v>-0.1214</v>
+        <v>0.1956000030040741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>